<commit_message>
documents code compare analysis dataset
</commit_message>
<xml_diff>
--- a/documents/code compare analysis.xlsx
+++ b/documents/code compare analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10800" windowHeight="9555"/>
+    <workbookView windowWidth="21600" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1733,8 +1733,8 @@
   <sheetPr/>
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="I46" workbookViewId="0">
+      <selection activeCell="K1" sqref="K$1:K$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14159292035398" defaultRowHeight="12.75"/>
@@ -1748,6 +1748,7 @@
     <col min="7" max="8" width="255.716814159292" customWidth="1"/>
     <col min="9" max="9" width="22.858407079646" customWidth="1"/>
     <col min="10" max="10" width="18.4247787610619" customWidth="1"/>
+    <col min="11" max="11" width="21.3805309734513" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1820,7 +1821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1851,8 +1852,11 @@
       <c r="J3">
         <v>-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1883,8 +1887,11 @@
       <c r="J4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1915,8 +1922,11 @@
       <c r="J5">
         <v>-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1947,8 +1957,11 @@
       <c r="J6">
         <v>-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1979,8 +1992,11 @@
       <c r="J7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2011,8 +2027,11 @@
       <c r="J8">
         <v>-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2043,8 +2062,11 @@
       <c r="J9">
         <v>-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2075,8 +2097,11 @@
       <c r="J10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2107,8 +2132,11 @@
       <c r="J11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2139,8 +2167,11 @@
       <c r="J12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2171,8 +2202,11 @@
       <c r="J13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2203,8 +2237,11 @@
       <c r="J14">
         <v>-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2235,8 +2272,11 @@
       <c r="J15">
         <v>-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2267,8 +2307,11 @@
       <c r="J16">
         <v>-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2299,8 +2342,11 @@
       <c r="J17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2331,8 +2377,11 @@
       <c r="J18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2363,8 +2412,11 @@
       <c r="J19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2395,8 +2447,11 @@
       <c r="J20">
         <v>-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2427,8 +2482,11 @@
       <c r="J21">
         <v>-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2459,8 +2517,11 @@
       <c r="J22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2491,8 +2552,11 @@
       <c r="J23">
         <v>-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2523,8 +2587,11 @@
       <c r="J24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2555,8 +2622,11 @@
       <c r="J25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2587,16 +2657,22 @@
       <c r="J26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="9:10">
+      <c r="K26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="9:11">
       <c r="I27">
         <v>1</v>
       </c>
       <c r="J27">
         <v>-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2627,8 +2703,11 @@
       <c r="J28">
         <v>-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2659,8 +2738,11 @@
       <c r="J29">
         <v>-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2691,8 +2773,11 @@
       <c r="J30">
         <v>-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2723,8 +2808,11 @@
       <c r="J31">
         <v>-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2755,8 +2843,11 @@
       <c r="J32">
         <v>-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2787,8 +2878,11 @@
       <c r="J33">
         <v>-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2819,8 +2913,11 @@
       <c r="J34">
         <v>-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2851,8 +2948,11 @@
       <c r="J35">
         <v>-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2883,8 +2983,11 @@
       <c r="J36">
         <v>-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2915,8 +3018,11 @@
       <c r="J37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2947,8 +3053,11 @@
       <c r="J38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2979,8 +3088,11 @@
       <c r="J39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3011,8 +3123,11 @@
       <c r="J40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3043,8 +3158,11 @@
       <c r="J41">
         <v>-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3075,8 +3193,11 @@
       <c r="J42">
         <v>-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3107,8 +3228,11 @@
       <c r="J43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3139,8 +3263,11 @@
       <c r="J44">
         <v>-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3171,8 +3298,11 @@
       <c r="J45">
         <v>-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3203,8 +3333,11 @@
       <c r="J46">
         <v>-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3235,8 +3368,11 @@
       <c r="J47">
         <v>-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3267,8 +3403,11 @@
       <c r="J48">
         <v>-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3299,8 +3438,11 @@
       <c r="J49">
         <v>-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3331,8 +3473,11 @@
       <c r="J50">
         <v>-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3363,8 +3508,11 @@
       <c r="J51">
         <v>-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3395,8 +3543,11 @@
       <c r="J52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3427,8 +3578,11 @@
       <c r="J53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3459,8 +3613,11 @@
       <c r="J54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3491,8 +3648,11 @@
       <c r="J55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3523,8 +3683,11 @@
       <c r="J56">
         <v>-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3555,8 +3718,11 @@
       <c r="J57">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3587,8 +3753,11 @@
       <c r="J58">
         <v>-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3619,8 +3788,11 @@
       <c r="J59">
         <v>-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3651,8 +3823,11 @@
       <c r="J60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3683,8 +3858,11 @@
       <c r="J61">
         <v>-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3713,6 +3891,9 @@
         <v>2</v>
       </c>
       <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
         <v>2</v>
       </c>
     </row>

</xml_diff>